<commit_message>
REPORTGEN-709: update CWE full excel reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CWE (2011) Top 25 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CWE (2011) Top 25 Full Detailed Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAE196E-C494-45EB-B1EC-93CCA145C01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5192289-DE89-4CBE-8E19-5C99744D012F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Application Name:</t>
   </si>
@@ -71,34 +71,88 @@
     <t>RepGen:TEXT;METRIC_TECHNICAL_DEBT</t>
   </si>
   <si>
-    <t>RepGen:TABLE;TECHNICAL_SIZING</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;TECHNO_LOC</t>
-  </si>
-  <si>
     <t>Application characteristics</t>
   </si>
   <si>
-    <t>CAST findings for CWE (2011) Top 25</t>
-  </si>
-  <si>
-    <t>CAST findings details for CWE (2011) Top 25</t>
-  </si>
-  <si>
     <t>CWE (2011) Top 25 Compliance details</t>
   </si>
   <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNO_LOC;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;TECHNICAL_SIZING;HEADER=NO</t>
+  </si>
+  <si>
+    <t>Quality Standard</t>
+  </si>
+  <si>
+    <t>Total Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Added Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Removed Vulnerabilities</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CWE-2011-Top25,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Remediation</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CWE-2011-Top25,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>Object Type</t>
+  </si>
+  <si>
+    <t>Violation Status</t>
+  </si>
+  <si>
+    <t>Associated Value</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Start Line</t>
+  </si>
+  <si>
+    <t>End Line</t>
+  </si>
+  <si>
     <t>Findings summary for CAST under CWE (2011) Top 25</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS;METRICS=CWE-2011-Top25,COUNT=-1</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=CWE-2011-Top25</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CWE-2011-Top25,MORE=true</t>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CWE-2011-Top25,COUNT=-1,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -305,7 +359,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -360,6 +414,16 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -419,7 +483,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>432089</xdr:colOff>
+      <xdr:colOff>16452</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>245918</xdr:rowOff>
     </xdr:to>
@@ -752,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O13"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -764,7 +828,7 @@
     <col min="2" max="2" width="75.33203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="16.109375" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -781,12 +845,12 @@
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -795,10 +859,10 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
@@ -811,10 +875,10 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
@@ -831,27 +895,59 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
+      <c r="D6" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>19</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -868,30 +964,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -901,26 +1023,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00038B0F-4F74-4ACF-8A7F-FE15A067CF76}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="175.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>